<commit_message>
Fix typo in sex item
</commit_message>
<xml_diff>
--- a/formr/CSV/bilexicon_lockdown_04_demo.xlsx
+++ b/formr/CSV/bilexicon_lockdown_04_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Documents\multilex\formr\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AF7179-1951-4887-A7B5-E2D07164501B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0037CE48-89C3-40B8-AE50-87067726B1BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-228" yWindow="12852" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-228" yWindow="12852" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -226,10 +226,10 @@
     <t>`r paste0(dplyr::case_when(bilexicon_lockdown_01_log$language == "catalan" ~paste0("Dona"), bilexicon_lockdown_01_log$language == "spanish" ~paste0("Mujer"), TRUE ~ paste0("Female")))`</t>
   </si>
   <si>
-    <t>`r paste0(dplyr::case_when(bilexicon_lockdown_01_log$language == "catalan" ~paste0("Home"), bilexicon_lockdown_01_log$language == "spanish" ~paste0("Hombre"), TRUE ~ paste0("Female")))`</t>
-  </si>
-  <si>
     <t>### `r paste0(dplyr::case_when(bilexicon_lockdown_01_log$language == "catalan" ~paste0("Sexe del bebé:"), bilexicon_lockdown_01_log$language == "spanish" ~paste0("Sexo del bebé:"), TRUE ~ paste0("Sex of the baby:")))`</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bilexicon_lockdown_01_log$language == "catalan" ~paste0("Home"), bilexicon_lockdown_01_log$language == "spanish" ~paste0("Hombre"), TRUE ~ paste0("Male")))`</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -715,7 +715,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
@@ -842,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -1004,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="61.2" x14ac:dyDescent="0.35">

</xml_diff>